<commit_message>
Messung 67mm vom 24.5.
</commit_message>
<xml_diff>
--- a/67mm_07_18/Auswertung.xlsx
+++ b/67mm_07_18/Auswertung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antony\Projects\pyt_Semi\67mm_07_18\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF70A922-2385-4519-AC92-CD0D9A29B4F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DECE30-2E4D-41C1-8622-71F636FBA20F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="11256" windowHeight="5568" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="11250" windowHeight="5565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="67mm_07_18" sheetId="1" r:id="rId1"/>
@@ -112,7 +112,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0000E+00"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="171" formatCode="0.0000000E+00"/>
+    <numFmt numFmtId="166" formatCode="0.0000000E+00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -310,10 +310,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -4243,20 +4243,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="97" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="97" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -4269,10 +4271,10 @@
       <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="17"/>
+      <c r="G1" s="18"/>
       <c r="H1" s="4"/>
       <c r="I1" t="s">
         <v>9</v>
@@ -4280,12 +4282,12 @@
       <c r="J1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="L1" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="17"/>
+      <c r="M1" s="18"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>0</v>
       </c>
@@ -4312,7 +4314,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0.14671072943450431</v>
       </c>
@@ -4340,16 +4342,16 @@
       <c r="J3">
         <v>14</v>
       </c>
-      <c r="L3" s="18">
+      <c r="L3" s="17">
         <f xml:space="preserve"> 0.004*A3^2 + 0.0011*A3 + 7*10^(-8)</f>
         <v>2.4754795490277207E-4</v>
       </c>
-      <c r="M3" s="18">
+      <c r="M3" s="17">
         <f xml:space="preserve"> 0.0069*A3^2 + 0.002*A3 + 8*10^(-8)</f>
         <v>4.4201732197431852E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0.13623139161775399</v>
       </c>
@@ -4377,16 +4379,16 @@
       <c r="J4">
         <v>13</v>
       </c>
-      <c r="L4" s="18">
+      <c r="L4" s="17">
         <f t="shared" ref="L4:L12" si="2" xml:space="preserve"> 0.004*A4^2 + 0.0011*A4 + 7*10^(-8)</f>
         <v>2.2416049902796879E-4</v>
       </c>
-      <c r="M4" s="18">
+      <c r="M4" s="17">
         <f t="shared" ref="M4:M12" si="3" xml:space="preserve"> 0.0069*A4^2 + 0.002*A4 + 8*10^(-8)</f>
         <v>4.0059982846406598E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0.12575205380100371</v>
       </c>
@@ -4414,16 +4416,16 @@
       <c r="J5">
         <v>12</v>
       </c>
-      <c r="L5" s="18">
+      <c r="L5" s="17">
         <f t="shared" si="2"/>
         <v>2.0165157532178621E-4</v>
       </c>
-      <c r="M5" s="18">
+      <c r="M5" s="17">
         <f t="shared" si="3"/>
         <v>3.606978029446841E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>0.1152727159842534</v>
       </c>
@@ -4451,16 +4453,16 @@
       <c r="J6">
         <v>11</v>
       </c>
-      <c r="L6" s="18">
+      <c r="L6" s="17">
         <f t="shared" si="2"/>
         <v>1.8002118378422413E-4</v>
       </c>
-      <c r="M6" s="18">
+      <c r="M6" s="17">
         <f t="shared" si="3"/>
         <v>3.2231124541617261E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>0.1047933781675031</v>
       </c>
@@ -4488,16 +4490,16 @@
       <c r="J7">
         <v>10</v>
       </c>
-      <c r="L7" s="18">
+      <c r="L7" s="17">
         <f t="shared" si="2"/>
         <v>1.5926932441528267E-4</v>
       </c>
-      <c r="M7" s="18">
+      <c r="M7" s="17">
         <f t="shared" si="3"/>
         <v>2.8544015587853169E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>9.431404035075279E-2</v>
       </c>
@@ -4525,16 +4527,16 @@
       <c r="J8">
         <v>9</v>
       </c>
-      <c r="L8" s="18">
+      <c r="L8" s="17">
         <f t="shared" si="2"/>
         <v>1.3939599721496179E-4</v>
       </c>
-      <c r="M8" s="18">
+      <c r="M8" s="17">
         <f t="shared" si="3"/>
         <v>2.5008453433176121E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8.3834702534002478E-2</v>
       </c>
@@ -4562,16 +4564,16 @@
       <c r="J9">
         <v>8</v>
       </c>
-      <c r="L9" s="18">
+      <c r="L9" s="17">
         <f t="shared" si="2"/>
         <v>1.2040120218326145E-4</v>
       </c>
-      <c r="M9" s="18">
+      <c r="M9" s="17">
         <f t="shared" si="3"/>
         <v>2.1624438077586129E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7.3355364717252167E-2</v>
       </c>
@@ -4599,16 +4601,16 @@
       <c r="J10">
         <v>7</v>
       </c>
-      <c r="L10" s="18">
+      <c r="L10" s="17">
         <f t="shared" si="2"/>
         <v>1.0228493932018173E-4</v>
       </c>
-      <c r="M10" s="18">
+      <c r="M10" s="17">
         <f t="shared" si="3"/>
         <v>1.8391969521083183E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>6.2876026900501855E-2</v>
       </c>
@@ -4636,16 +4638,16 @@
       <c r="J11">
         <v>6</v>
       </c>
-      <c r="L11" s="18">
+      <c r="L11" s="17">
         <f t="shared" si="2"/>
         <v>8.5047208625722574E-5</v>
       </c>
-      <c r="M11" s="18">
+      <c r="M11" s="17">
         <f t="shared" si="3"/>
         <v>1.5311047763667289E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>5.2396689083751551E-2</v>
       </c>
@@ -4673,23 +4675,23 @@
       <c r="J12">
         <v>5</v>
       </c>
-      <c r="L12" s="18">
+      <c r="L12" s="17">
         <f t="shared" si="2"/>
         <v>6.8688010099884027E-5</v>
       </c>
-      <c r="M12" s="18">
+      <c r="M12" s="17">
         <f t="shared" si="3"/>
         <v>1.2381672805338449E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
       <c r="D13" s="16"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
         <v>6</v>
       </c>
@@ -4700,7 +4702,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F16">
         <v>2.9499999999999998E-2</v>
       </c>

</xml_diff>